<commit_message>
Get row count function added
</commit_message>
<xml_diff>
--- a/DataFiles/student-data.xlsx
+++ b/DataFiles/student-data.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14845\Dropbox\Code\Reusable\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247566DD-1022-49C5-B0B0-A79DFF8DE226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8459CA0B-FAD3-4EDD-A3B3-8E028DAC400E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="student-data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>

</xml_diff>